<commit_message>
Added new library preparation kits and preparation instrument kits
Closes #16
</commit_message>
<xml_diff>
--- a/rnaseq/latest/rnaseq.xlsx
+++ b/rnaseq/latest/rnaseq.xlsx
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="503">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -723,127 +723,1054 @@
     <t>https://identifiers.org/RRID:SCR_008452</t>
   </si>
   <si>
+    <t>Zeiss Microscopy</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023607</t>
+  </si>
+  <si>
+    <t>Standard BioTools (Fluidigm)</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023606</t>
+  </si>
+  <si>
+    <t>GE Healthcare</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_000004</t>
+  </si>
+  <si>
+    <t>Sciex</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023651</t>
+  </si>
+  <si>
+    <t>Bruker</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_017365</t>
+  </si>
+  <si>
+    <t>Akoya Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023774</t>
+  </si>
+  <si>
+    <t>Evident Scientific (Olympus)</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024782</t>
+  </si>
+  <si>
+    <t>Keyence</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023604</t>
+  </si>
+  <si>
+    <t>Leica Biosystems</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023603</t>
+  </si>
+  <si>
+    <t>NanoString</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023912</t>
+  </si>
+  <si>
+    <t>Hamamatsu</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_017105</t>
+  </si>
+  <si>
+    <t>Andor</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023609</t>
+  </si>
+  <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
+    <t>Illumina</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_010233</t>
+  </si>
+  <si>
+    <t>Motic</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024856</t>
+  </si>
+  <si>
+    <t>Ionpath</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023605</t>
+  </si>
+  <si>
+    <t>acquisition_instrument_model</t>
+  </si>
+  <si>
+    <t>SCN400</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023611</t>
+  </si>
+  <si>
+    <t>STELLARIS 5</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024663</t>
+  </si>
+  <si>
+    <t>BZ-X710</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_017202</t>
+  </si>
+  <si>
+    <t>NanoZoomer S210</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023760</t>
+  </si>
+  <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
+    <t>Axio Observer 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023694</t>
+  </si>
+  <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
+    <t>IN Cell Analyzer 2200</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023616</t>
+  </si>
+  <si>
+    <t>PhenoImager Fusion</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023274</t>
+  </si>
+  <si>
+    <t>DM6 B</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024857</t>
+  </si>
+  <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 2.0</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023773</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024448</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
+    <t>Orbitrap Fusion Lumos Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020562</t>
+  </si>
+  <si>
+    <t>Resolve Biosciences Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024449</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>MALDI timsTOF Flex Prototype</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023615</t>
+  </si>
+  <si>
+    <t>TissueScope LE Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024995</t>
+  </si>
+  <si>
+    <t>VS200 Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024783</t>
+  </si>
+  <si>
+    <t>Axio Observer 5</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023692</t>
+  </si>
+  <si>
+    <t>Axio Observer 3</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023693</t>
+  </si>
+  <si>
+    <t>HiSeq 2500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016383</t>
+  </si>
+  <si>
+    <t>Orbitrap Eclipse Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023618</t>
+  </si>
+  <si>
+    <t>Q Exactive UHMR</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020571</t>
+  </si>
+  <si>
+    <t>NextSeq 2000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023614</t>
+  </si>
+  <si>
+    <t>NovaSeq 6000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016387</t>
+  </si>
+  <si>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020565</t>
+  </si>
+  <si>
+    <t>Zyla 4.2 sCMOS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023610</t>
+  </si>
+  <si>
+    <t>HiSeq 4000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016386</t>
+  </si>
+  <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
+    <t>QTRAP 5500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020517</t>
+  </si>
+  <si>
+    <t>BZ-X800</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023617</t>
+  </si>
+  <si>
+    <t>Aperio AT2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021256</t>
+  </si>
+  <si>
+    <t>MIBIscope</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023613</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_014983</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>NanoZoomer S60</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023762</t>
+  </si>
+  <si>
+    <t>CosMx Spatial Molecular Imager</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023909</t>
+  </si>
+  <si>
+    <t>Hyperion Imaging System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023195</t>
+  </si>
+  <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016381</t>
+  </si>
+  <si>
+    <t>Digital Spatial Profiler</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021660</t>
+  </si>
+  <si>
+    <t>Axio Scan.Z1</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020927</t>
+  </si>
+  <si>
+    <t>Q Exactive HF</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020558</t>
+  </si>
+  <si>
+    <t>Xenium Analyzer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023910</t>
+  </si>
+  <si>
+    <t>source_storage_duration_value</t>
+  </si>
+  <si>
+    <t>source_storage_duration_unit</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000032</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000035</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000036</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000033</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000031</t>
+  </si>
+  <si>
+    <t>time_since_acquisition_instrument_calibration_value</t>
+  </si>
+  <si>
+    <t>time_since_acquisition_instrument_calibration_unit</t>
+  </si>
+  <si>
+    <t>contributors_path</t>
+  </si>
+  <si>
+    <t>data_path</t>
+  </si>
+  <si>
+    <t>barcode_offset</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0,38,76</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>1,27</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>10,48,86</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>barcode_read</t>
+  </si>
+  <si>
+    <t>Read 1 (R1)</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C172301</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
+  </si>
+  <si>
+    <t>Read 2 (R2)</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C172302</t>
+  </si>
+  <si>
+    <t>barcode_size</t>
+  </si>
+  <si>
+    <t>8,6</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>8,8,8</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>umi_offset</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>umi_read</t>
+  </si>
+  <si>
+    <t>umi_size</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>assay_input_entity</t>
+  </si>
+  <si>
+    <t>single nucleus</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000269</t>
+  </si>
+  <si>
+    <t>single cell</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000268</t>
+  </si>
+  <si>
+    <t>tissue (bulk)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000267</t>
+  </si>
+  <si>
+    <t>spot</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000270</t>
+  </si>
+  <si>
+    <t>area of interest</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000271</t>
+  </si>
+  <si>
+    <t>number_of_input_cells_or_nuclei</t>
+  </si>
+  <si>
+    <t>amount_of_input_analyte_value</t>
+  </si>
+  <si>
+    <t>amount_of_input_analyte_unit</t>
+  </si>
+  <si>
+    <t>ng</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000024</t>
+  </si>
+  <si>
+    <t>ug</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000023</t>
+  </si>
+  <si>
+    <t>library_adapter_sequence</t>
+  </si>
+  <si>
+    <t>library_average_fragment_size</t>
+  </si>
+  <si>
+    <t>library_input_amount_value</t>
+  </si>
+  <si>
+    <t>library_input_amount_unit</t>
+  </si>
+  <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000101</t>
+  </si>
+  <si>
+    <t>library_output_amount_value</t>
+  </si>
+  <si>
+    <t>library_output_amount_unit</t>
+  </si>
+  <si>
+    <t>library_concentration_value</t>
+  </si>
+  <si>
+    <t>library_concentration_unit</t>
+  </si>
+  <si>
+    <t>ng/ul</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0010050</t>
+  </si>
+  <si>
+    <t>nM</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000065</t>
+  </si>
+  <si>
+    <t>library_layout</t>
+  </si>
+  <si>
+    <t>single-end</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002481</t>
+  </si>
+  <si>
+    <t>paired-end</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000722</t>
+  </si>
+  <si>
+    <t>number_of_iterations_of_cdna_amplification</t>
+  </si>
+  <si>
+    <t>number_of_pcr_cycles_for_indexing</t>
+  </si>
+  <si>
+    <t>library_preparation_kit</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 8 rxns; PN 1000370</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000336</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq Stranded mRNA Library Prep (96 samples); PN 20020595</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000344</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 4 rxns; PN 1000298</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000366</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 4 rxns; PN 1000265</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000340</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000261</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; Evercode WT v2 Kit, 48 rxns; PN ECW02030</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000341</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 16 rxns; PN 1000263</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000339</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns PN 1000092</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 16 rxns; PN 1000268</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000337</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000335</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN 120267</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000299</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Mouse Transcriptome, 4 rxns; PN 1000339</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000355</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000322</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq Stranded mRNA Library Prep (48 samples); PN 20020594</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000343</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 24 rxns; PN 1000290</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000365</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 4 rxns; PN 1000269</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000338</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3’ GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000342</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000321</t>
+  </si>
+  <si>
+    <t>sample_indexing_kit</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq RNA CD Index Plate (96 Indexes, 96 Samples); PN 20019792</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000349</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq RNA Single Indexes Set A (12 Indexes, 48 Samples); PN 20020492</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000347</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq RNA Single Indexes Set B (12 Indexes, 48 Samples); PN 20020493</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000348</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-AB</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000356</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-CD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000357</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-EF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000358</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-GH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000359</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; Fragmentation Reagents; PN WX100</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000345</t>
+  </si>
+  <si>
+    <t>Integrated DNA Technologies: Custom DNA Oligos</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000351</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; UDI Plate - WT; PN UDI1001</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000346</t>
+  </si>
+  <si>
+    <t>10X Genomics; Dual Index Kit TS, Set A; PN 1000251</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000282</t>
+  </si>
+  <si>
+    <t>Illumina; IDT for Illumina - TruSeq RNA UD Indexes v2 (96 Indexes, 96 Samples); PN 20040871</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000350</t>
+  </si>
+  <si>
+    <t>10X Genomics; Single Index Kit N, Set A (96 rxn); PN 1000212</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000252</t>
+  </si>
+  <si>
+    <t>10X Genomics; Dual Index Kit TT, Set A (96 rxn); PN 1000215</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000253</t>
+  </si>
+  <si>
+    <t>sample_indexing_set</t>
+  </si>
+  <si>
+    <t>is_technical_replicate</t>
+  </si>
+  <si>
+    <t>expected_entity_capture_count</t>
+  </si>
+  <si>
+    <t>sequencing_reagent_kit</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (100 Cycle); PN 20104703</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000286</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (300 Cycle); PN 20104705</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000288</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (200 Cycles); PN 20028318</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000360</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (100 Cycles); PN 20028319</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000257</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 SP Reagent v1.5 Kit (100 Cycles); PN 20028401</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000256</t>
+  </si>
+  <si>
+    <t>Illumina; HiSeq 3000/4000 PE Cluster Kit PE-410-1001; PN 1000283</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (300 Cycles); PN 20046813</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000353</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 2000 P3 Reagents Kit (100 Cycles); PN 20040559</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000361</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (300 Cycles); PN 20028317</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000318</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (100 Cycles); PN 20046811</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000323</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 2000 P3 Reagent Kit (300 Cycles); PN 20040561</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000354</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000284</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (200 Cycles); PN 20046812</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000352</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 500/550 Hi Output Kit 150 Cycles; v2.5; PN 20024907</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000255</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent Kit (200 Cycles); PN 20012864</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000313</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S4 Reagent v1.5 Kit (200 Cycles); PN 20028313</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000259</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (200 Cycle); PN 20104704</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles); PN 20028312</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000319</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 10B Reagent Kit (300 Cycle); PN 20085594</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000283</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 10B Reagent Kit (100 Cycle); PN 20085596</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000285</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S2 Reagent v1.5 Kit (100 Cycles); PN 20028316</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000258</t>
+  </si>
+  <si>
+    <t>sequencing_read_format</t>
+  </si>
+  <si>
+    <t>sequencing_batch_id</t>
+  </si>
+  <si>
+    <t>capture_batch_id</t>
+  </si>
+  <si>
+    <t>preparation_instrument_vendor</t>
+  </si>
+  <si>
     <t>Roche Diagnostics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_025096</t>
   </si>
   <si>
-    <t>Zeiss Microscopy</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023607</t>
-  </si>
-  <si>
-    <t>Standard BioTools (Fluidigm)</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023606</t>
-  </si>
-  <si>
-    <t>Sciex</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023651</t>
-  </si>
-  <si>
-    <t>Bruker</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_017365</t>
-  </si>
-  <si>
-    <t>Akoya Biosciences</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023774</t>
-  </si>
-  <si>
-    <t>Evident Scientific (Olympus)</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024782</t>
-  </si>
-  <si>
-    <t>Keyence</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023604</t>
-  </si>
-  <si>
-    <t>Leica Biosystems</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023603</t>
-  </si>
-  <si>
-    <t>NanoString</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023912</t>
-  </si>
-  <si>
-    <t>Hamamatsu</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_017105</t>
-  </si>
-  <si>
-    <t>Andor</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023609</t>
-  </si>
-  <si>
-    <t>Huron Digital Pathology</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024996</t>
-  </si>
-  <si>
-    <t>Illumina</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_010233</t>
-  </si>
-  <si>
-    <t>Motic</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024856</t>
-  </si>
-  <si>
-    <t>Ionpath</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023605</t>
-  </si>
-  <si>
-    <t>acquisition_instrument_model</t>
-  </si>
-  <si>
-    <t>SCN400</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023611</t>
-  </si>
-  <si>
-    <t>STELLARIS 5</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024663</t>
-  </si>
-  <si>
-    <t>BZ-X710</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_017202</t>
-  </si>
-  <si>
-    <t>MoticEasyScan One</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024855</t>
+    <t>HTX Technologies</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023734</t>
+  </si>
+  <si>
+    <t>10x Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023672</t>
+  </si>
+  <si>
+    <t>SunChrom</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023908</t>
+  </si>
+  <si>
+    <t>preparation_instrument_model</t>
+  </si>
+  <si>
+    <t>Sublimator</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023729</t>
   </si>
   <si>
     <t>EVOS M7000</t>
@@ -852,40 +1779,40 @@
     <t>https://identifiers.org/RRID:SCR_025070</t>
   </si>
   <si>
-    <t>NovaSeq X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024569</t>
-  </si>
-  <si>
-    <t>NanoZoomer 2.0-HT</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021658</t>
-  </si>
-  <si>
-    <t>Lightsheet 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024448</t>
-  </si>
-  <si>
-    <t>Phenocycler-Fusion 1.0</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
-  </si>
-  <si>
-    <t>DNBSEQ-T7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024847</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+    <t>Chromium Controller</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_019326</t>
+  </si>
+  <si>
+    <t>Chromium X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024537</t>
+  </si>
+  <si>
+    <t>AutoStainer XL</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023957</t>
+  </si>
+  <si>
+    <t>Visium CytAssist</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024570</t>
+  </si>
+  <si>
+    <t>SunCollect Sprayer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023907</t>
+  </si>
+  <si>
+    <t>M3+ Sprayer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
     <t>Discovery Ultra</t>
@@ -894,915 +1821,6 @@
     <t>https://identifiers.org/RRID:SCR_025097</t>
   </si>
   <si>
-    <t>Q Exactive UHMR</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020571</t>
-  </si>
-  <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020565</t>
-  </si>
-  <si>
-    <t>Zyla 4.2 sCMOS</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023610</t>
-  </si>
-  <si>
-    <t>Custom: Multiphoton</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
-  </si>
-  <si>
-    <t>QTRAP 5500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020517</t>
-  </si>
-  <si>
-    <t>BZ-X800</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023617</t>
-  </si>
-  <si>
-    <t>NextSeq 500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_014983</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
-    <t>Hyperion Imaging System</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023195</t>
-  </si>
-  <si>
-    <t>NovaSeq X Plus</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024568</t>
-  </si>
-  <si>
-    <t>NanoZoomer-SQ</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023763</t>
-  </si>
-  <si>
-    <t>NextSeq 550</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016381</t>
-  </si>
-  <si>
-    <t>Digital Spatial Profiler</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021660</t>
-  </si>
-  <si>
-    <t>NanoZoomer S210</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023760</t>
-  </si>
-  <si>
-    <t>Axio Observer 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023694</t>
-  </si>
-  <si>
-    <t>IN Cell Analyzer 2200</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023616</t>
-  </si>
-  <si>
-    <t>PhenoImager Fusion</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023274</t>
-  </si>
-  <si>
-    <t>DM6 B</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024857</t>
-  </si>
-  <si>
-    <t>Phenocycler-Fusion 2.0</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023773</t>
-  </si>
-  <si>
-    <t>Orbitrap Fusion Lumos Tribrid</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020562</t>
-  </si>
-  <si>
-    <t>Resolve Biosciences Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024449</t>
-  </si>
-  <si>
-    <t>MALDI timsTOF Flex Prototype</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023615</t>
-  </si>
-  <si>
-    <t>TissueScope LE Slide Scanner</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024995</t>
-  </si>
-  <si>
-    <t>VS200 Slide Scanner</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024783</t>
-  </si>
-  <si>
-    <t>Axio Observer 5</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023692</t>
-  </si>
-  <si>
-    <t>Axio Observer 3</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023693</t>
-  </si>
-  <si>
-    <t>HiSeq 2500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016383</t>
-  </si>
-  <si>
-    <t>Orbitrap Eclipse Tribrid</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023618</t>
-  </si>
-  <si>
-    <t>NextSeq 2000</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023614</t>
-  </si>
-  <si>
-    <t>NovaSeq 6000</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016387</t>
-  </si>
-  <si>
-    <t>HiSeq 4000</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016386</t>
-  </si>
-  <si>
-    <t>Aperio AT2</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021256</t>
-  </si>
-  <si>
-    <t>MIBIscope</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023613</t>
-  </si>
-  <si>
-    <t>NanoZoomer S60</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023762</t>
-  </si>
-  <si>
-    <t>CosMx Spatial Molecular Imager</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023909</t>
-  </si>
-  <si>
-    <t>Axio Scan.Z1</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020927</t>
-  </si>
-  <si>
-    <t>Q Exactive HF</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020558</t>
-  </si>
-  <si>
-    <t>Xenium Analyzer</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023910</t>
-  </si>
-  <si>
-    <t>source_storage_duration_value</t>
-  </si>
-  <si>
-    <t>source_storage_duration_unit</t>
-  </si>
-  <si>
-    <t>hour</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000032</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000035</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000036</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000033</t>
-  </si>
-  <si>
-    <t>minute</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000031</t>
-  </si>
-  <si>
-    <t>time_since_acquisition_instrument_calibration_value</t>
-  </si>
-  <si>
-    <t>time_since_acquisition_instrument_calibration_unit</t>
-  </si>
-  <si>
-    <t>contributors_path</t>
-  </si>
-  <si>
-    <t>data_path</t>
-  </si>
-  <si>
-    <t>barcode_offset</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0,38,76</t>
-  </si>
-  <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
-    <t>1,27</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>10,48,86</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>barcode_read</t>
-  </si>
-  <si>
-    <t>Read 1 (R1)</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C172301</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
-  </si>
-  <si>
-    <t>Read 2 (R2)</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C172302</t>
-  </si>
-  <si>
-    <t>barcode_size</t>
-  </si>
-  <si>
-    <t>8,6</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>8,8,8</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>umi_offset</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>umi_read</t>
-  </si>
-  <si>
-    <t>umi_size</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>assay_input_entity</t>
-  </si>
-  <si>
-    <t>single nucleus</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000269</t>
-  </si>
-  <si>
-    <t>single cell</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000268</t>
-  </si>
-  <si>
-    <t>tissue (bulk)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000267</t>
-  </si>
-  <si>
-    <t>spot</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000270</t>
-  </si>
-  <si>
-    <t>area of interest</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000271</t>
-  </si>
-  <si>
-    <t>number_of_input_cells_or_nuclei</t>
-  </si>
-  <si>
-    <t>amount_of_input_analyte_value</t>
-  </si>
-  <si>
-    <t>amount_of_input_analyte_unit</t>
-  </si>
-  <si>
-    <t>ng</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000024</t>
-  </si>
-  <si>
-    <t>ug</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000023</t>
-  </si>
-  <si>
-    <t>library_adapter_sequence</t>
-  </si>
-  <si>
-    <t>library_average_fragment_size</t>
-  </si>
-  <si>
-    <t>library_input_amount_value</t>
-  </si>
-  <si>
-    <t>library_input_amount_unit</t>
-  </si>
-  <si>
-    <t>ul</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000101</t>
-  </si>
-  <si>
-    <t>library_output_amount_value</t>
-  </si>
-  <si>
-    <t>library_output_amount_unit</t>
-  </si>
-  <si>
-    <t>library_concentration_value</t>
-  </si>
-  <si>
-    <t>library_concentration_unit</t>
-  </si>
-  <si>
-    <t>ng/ul</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0010050</t>
-  </si>
-  <si>
-    <t>nM</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000065</t>
-  </si>
-  <si>
-    <t>library_layout</t>
-  </si>
-  <si>
-    <t>single-end</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0002481</t>
-  </si>
-  <si>
-    <t>paired-end</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0000722</t>
-  </si>
-  <si>
-    <t>number_of_iterations_of_cdna_amplification</t>
-  </si>
-  <si>
-    <t>number_of_pcr_cycles_for_indexing</t>
-  </si>
-  <si>
-    <t>library_preparation_kit</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 8 rxns; PN 1000370</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000336</t>
-  </si>
-  <si>
-    <t>Illumina; TruSeq Stranded mRNA Library Prep (96 samples); PN 20020595</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000344</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 4 rxns; PN 1000265</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000340</t>
-  </si>
-  <si>
-    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000261</t>
-  </si>
-  <si>
-    <t>Parse Biosciences; Evercode WT v2 Kit, 48 rxns; PN ECW02030</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000341</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 16 rxns; PN 1000263</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000339</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns PN 1000092</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
-  </si>
-  <si>
-    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 16 rxns; PN 1000268</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000337</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000335</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN 120267</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000299</t>
-  </si>
-  <si>
-    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Mouse Transcriptome, 4 rxns; PN 1000339</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000355</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
-  </si>
-  <si>
-    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000322</t>
-  </si>
-  <si>
-    <t>Illumina; TruSeq Stranded mRNA Library Prep (48 samples); PN 20020594</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000343</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 4 rxns; PN 1000269</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000338</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3’ GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
-  </si>
-  <si>
-    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
-  </si>
-  <si>
-    <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000342</t>
-  </si>
-  <si>
-    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000321</t>
-  </si>
-  <si>
-    <t>sample_indexing_kit</t>
-  </si>
-  <si>
-    <t>Illumina; TruSeq RNA CD Index Plate (96 Indexes, 96 Samples); PN 20019792</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000349</t>
-  </si>
-  <si>
-    <t>Illumina; TruSeq RNA Single Indexes Set A (12 Indexes, 48 Samples); PN 20020492</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000347</t>
-  </si>
-  <si>
-    <t>Illumina; TruSeq RNA Single Indexes Set B (12 Indexes, 48 Samples); PN 20020493</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000348</t>
-  </si>
-  <si>
-    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-AB</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000356</t>
-  </si>
-  <si>
-    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-CD</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000357</t>
-  </si>
-  <si>
-    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-EF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000358</t>
-  </si>
-  <si>
-    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-GH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000359</t>
-  </si>
-  <si>
-    <t>Parse Biosciences; Fragmentation Reagents; PN WX100</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000345</t>
-  </si>
-  <si>
-    <t>Integrated DNA Technologies: Custom DNA Oligos</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000351</t>
-  </si>
-  <si>
-    <t>Parse Biosciences; UDI Plate - WT; PN UDI1001</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000346</t>
-  </si>
-  <si>
-    <t>10X Genomics; Dual Index Kit TS, Set A; PN 1000251</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000282</t>
-  </si>
-  <si>
-    <t>Illumina; IDT for Illumina - TruSeq RNA UD Indexes v2 (96 Indexes, 96 Samples); PN 20040871</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000350</t>
-  </si>
-  <si>
-    <t>10X Genomics; Single Index Kit N, Set A (96 rxn); PN 1000212</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000252</t>
-  </si>
-  <si>
-    <t>10X Genomics; Dual Index Kit TT, Set A (96 rxn); PN 1000215</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000253</t>
-  </si>
-  <si>
-    <t>sample_indexing_set</t>
-  </si>
-  <si>
-    <t>is_technical_replicate</t>
-  </si>
-  <si>
-    <t>expected_entity_capture_count</t>
-  </si>
-  <si>
-    <t>sequencing_reagent_kit</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (100 Cycle); PN 20104703</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000286</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (300 Cycle); PN 20104705</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000288</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (200 Cycles); PN 20028318</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000360</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (100 Cycles); PN 20028319</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000257</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 SP Reagent v1.5 Kit (100 Cycles); PN 20028401</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000256</t>
-  </si>
-  <si>
-    <t>Illumina; HiSeq 3000/4000 PE Cluster Kit PE-410-1001; PN 1000283</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
-  </si>
-  <si>
-    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (300 Cycles); PN 20046813</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000353</t>
-  </si>
-  <si>
-    <t>Illumina; NextSeq 2000 P3 Reagents Kit (100 Cycles); PN 20040559</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000361</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (300 Cycles); PN 20028317</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000318</t>
-  </si>
-  <si>
-    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (100 Cycles); PN 20046811</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000323</t>
-  </si>
-  <si>
-    <t>Illumina; NextSeq 2000 P3 Reagent Kit (300 Cycles); PN 20040561</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000354</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000284</t>
-  </si>
-  <si>
-    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (200 Cycles); PN 20046812</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000352</t>
-  </si>
-  <si>
-    <t>Illumina; NextSeq 500/550 Hi Output Kit 150 Cycles; v2.5; PN 20024907</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000255</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S1 Reagent Kit (200 Cycles); PN 20012864</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000313</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S4 Reagent v1.5 Kit (200 Cycles); PN 20028313</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000259</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (200 Cycle); PN 20104704</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles); PN 20028312</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000319</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq X Series 10B Reagent Kit (300 Cycle); PN 20085594</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000283</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq X Series 10B Reagent Kit (100 Cycle); PN 20085596</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000285</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S2 Reagent v1.5 Kit (100 Cycles); PN 20028316</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000258</t>
-  </si>
-  <si>
-    <t>sequencing_read_format</t>
-  </si>
-  <si>
-    <t>sequencing_batch_id</t>
-  </si>
-  <si>
-    <t>capture_batch_id</t>
-  </si>
-  <si>
-    <t>preparation_instrument_vendor</t>
-  </si>
-  <si>
-    <t>HTX Technologies</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023734</t>
-  </si>
-  <si>
-    <t>10x Genomics</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023672</t>
-  </si>
-  <si>
-    <t>SunChrom</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023908</t>
-  </si>
-  <si>
-    <t>preparation_instrument_model</t>
-  </si>
-  <si>
-    <t>Sublimator</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023729</t>
-  </si>
-  <si>
-    <t>Chromium Controller</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_019326</t>
-  </si>
-  <si>
-    <t>Chromium X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024537</t>
-  </si>
-  <si>
-    <t>AutoStainer XL</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023957</t>
-  </si>
-  <si>
-    <t>Visium CytAssist</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024570</t>
-  </si>
-  <si>
-    <t>SunCollect Sprayer</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023907</t>
-  </si>
-  <si>
-    <t>M3+ Sprayer</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023731</t>
-  </si>
-  <si>
     <t>ST5020 Multistainer</t>
   </si>
   <si>
@@ -1830,18 +1848,30 @@
     <t>preparation_instrument_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip K Single Cell Kit, 48 rxns; PN 1000286</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000367</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium FFPE Reagent Kit v2-Small, PN 1000436</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000324</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Next GEM Chip Q Single Cell Kit, 16 rxns; PN 1000422</t>
+    <t>10X Genomics; Chromium Next GEM Chip Q Single Cell Kit, 16 rxns; PN 1000422</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000325</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip K Single Cell Kit, 16 rxns; PN 1000287</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000368</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1860,7 +1890,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-18T09:17:36-07:00</t>
+    <t>2024-03-20T10:47:13-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2064,88 +2094,88 @@
         <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="K1" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="L1" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="M1" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="N1" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="O1" t="s" s="1">
         <v>256</v>
       </c>
-      <c r="L1" t="s" s="1">
-        <v>257</v>
-      </c>
-      <c r="M1" t="s" s="1">
-        <v>258</v>
-      </c>
-      <c r="N1" t="s" s="1">
-        <v>259</v>
-      </c>
-      <c r="O1" t="s" s="1">
-        <v>260</v>
-      </c>
       <c r="P1" t="s" s="1">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="T1" t="s" s="1">
+        <v>279</v>
+      </c>
+      <c r="U1" t="s" s="1">
         <v>283</v>
       </c>
-      <c r="U1" t="s" s="1">
-        <v>287</v>
-      </c>
       <c r="V1" t="s" s="1">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="AA1" t="s" s="1">
+        <v>303</v>
+      </c>
+      <c r="AB1" t="s" s="1">
+        <v>304</v>
+      </c>
+      <c r="AC1" t="s" s="1">
         <v>307</v>
       </c>
-      <c r="AB1" t="s" s="1">
+      <c r="AD1" t="s" s="1">
         <v>308</v>
       </c>
-      <c r="AC1" t="s" s="1">
-        <v>311</v>
-      </c>
-      <c r="AD1" t="s" s="1">
-        <v>312</v>
-      </c>
       <c r="AE1" t="s" s="1">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="AK1" t="s" s="1">
         <v>371</v>
@@ -2175,13 +2205,13 @@
         <v>449</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>484</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2">
@@ -2189,7 +2219,7 @@
         <v>52</v>
       </c>
       <c r="AV2" t="s" s="49">
-        <v>485</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -2207,7 +2237,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$50</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2292,7 +2322,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$22</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$24</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$15</formula1>
@@ -2308,13 +2338,13 @@
       <formula1>'sequencing_reagent_kit'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
+      <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AT2:AT1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$15</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$17</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$4</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2333,26 +2363,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2370,32 +2400,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2413,22 +2443,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2446,26 +2476,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2483,27 +2513,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2521,42 +2551,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2574,18 +2604,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2603,18 +2633,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2632,18 +2662,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2661,18 +2691,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2975,18 +3005,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2996,7 +3026,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3004,177 +3034,193 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>367</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
         <v>369</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B24" t="s" s="0">
         <v>370</v>
       </c>
     </row>
@@ -3201,10 +3247,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
@@ -3522,7 +3568,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3546,34 +3592,34 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>450</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>451</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>131</v>
+        <v>452</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>132</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7">
@@ -3582,6 +3628,22 @@
       </c>
       <c r="B7" t="s" s="0">
         <v>455</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>456</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -3591,7 +3653,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3599,122 +3661,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>195</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>182</v>
+        <v>463</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>183</v>
+        <v>464</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>461</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>462</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>478</v>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>481</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>483</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -3724,7 +3802,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3732,34 +3810,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>486</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>480</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>481</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>483</v>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>492</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -3783,16 +3877,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>486</v>
+        <v>496</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>489</v>
+        <v>499</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>491</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2">
@@ -3800,13 +3894,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>492</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -4129,7 +4223,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4517,22 +4611,6 @@
       </c>
       <c r="B48" t="s" s="0">
         <v>239</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="0">
-        <v>240</v>
-      </c>
-      <c r="B49" t="s" s="0">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="0">
-        <v>242</v>
-      </c>
-      <c r="B50" t="s" s="0">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4550,42 +4628,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4603,26 +4681,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4640,37 +4718,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix a typo in the library preparation kit
</commit_message>
<xml_diff>
--- a/rnaseq/latest/rnaseq.xlsx
+++ b/rnaseq/latest/rnaseq.xlsx
@@ -1449,6 +1449,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000355</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
   </si>
   <si>
@@ -1479,12 +1485,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000338</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3’ GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
-  </si>
-  <si>
     <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
   </si>
   <si>
@@ -1890,7 +1890,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-20T10:47:13-07:00</t>
+    <t>2024-03-21T13:34:28-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -3826,10 +3826,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Added '10,48,78' in the barcode offset
Closes #18
</commit_message>
<xml_diff>
--- a/rnaseq/latest/rnaseq.xlsx
+++ b/rnaseq/latest/rnaseq.xlsx
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="510">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -840,30 +840,144 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024448</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>Q Exactive UHMR</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020571</t>
+  </si>
+  <si>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020565</t>
+  </si>
+  <si>
+    <t>Zyla 4.2 sCMOS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023610</t>
+  </si>
+  <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
+    <t>QTRAP 5500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020517</t>
+  </si>
+  <si>
+    <t>BZ-X800</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023617</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_014983</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>Hyperion Imaging System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023195</t>
+  </si>
+  <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016381</t>
+  </si>
+  <si>
+    <t>Digital Spatial Profiler</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021660</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
-    <t>MoticEasyScan One</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024855</t>
-  </si>
-  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
-    <t>NovaSeq X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024569</t>
-  </si>
-  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -882,36 +996,12 @@
     <t>https://identifiers.org/RRID:SCR_024857</t>
   </si>
   <si>
-    <t>NanoZoomer 2.0-HT</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021658</t>
-  </si>
-  <si>
     <t>Phenocycler-Fusion 2.0</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023773</t>
   </si>
   <si>
-    <t>Lightsheet 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024448</t>
-  </si>
-  <si>
-    <t>Phenocycler-Fusion 1.0</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
-  </si>
-  <si>
-    <t>DNBSEQ-T7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024847</t>
-  </si>
-  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -924,12 +1014,6 @@
     <t>https://identifiers.org/RRID:SCR_024449</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
-  </si>
-  <si>
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
@@ -972,12 +1056,6 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
-    <t>Q Exactive UHMR</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020571</t>
-  </si>
-  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -990,42 +1068,12 @@
     <t>https://identifiers.org/RRID:SCR_016387</t>
   </si>
   <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020565</t>
-  </si>
-  <si>
-    <t>Zyla 4.2 sCMOS</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023610</t>
-  </si>
-  <si>
     <t>HiSeq 4000</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
-    <t>Custom: Multiphoton</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
-  </si>
-  <si>
-    <t>QTRAP 5500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020517</t>
-  </si>
-  <si>
-    <t>BZ-X800</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023617</t>
-  </si>
-  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1038,18 +1086,6 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
-    <t>NextSeq 500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_014983</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1062,36 +1098,6 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
-    <t>Hyperion Imaging System</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023195</t>
-  </si>
-  <si>
-    <t>NovaSeq X Plus</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024568</t>
-  </si>
-  <si>
-    <t>NanoZoomer-SQ</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023763</t>
-  </si>
-  <si>
-    <t>NextSeq 550</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016381</t>
-  </si>
-  <si>
-    <t>Digital Spatial Profiler</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021660</t>
-  </si>
-  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1179,6 +1185,9 @@
     <t>10,48,86</t>
   </si>
   <si>
+    <t>10,48,78</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
@@ -1365,78 +1374,120 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000336</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 4 rxns; PN 1000298</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000366</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000261</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; Evercode WT v2 Kit, 48 rxns; PN ECW02030</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000341</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 16 rxns; PN 1000263</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000339</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 16 rxns; PN 1000268</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000337</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000335</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000322</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq Stranded mRNA Library Prep (48 samples); PN 20020594</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000343</t>
+  </si>
+  <si>
+    <t>10X Genomics; Automated Library Construction Kit, 24 rxns; PN 1000428</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000374</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 24 rxns; PN 1000290</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000365</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000342</t>
+  </si>
+  <si>
     <t>Illumina; TruSeq Stranded mRNA Library Prep (96 samples); PN 20020595</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000344</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 4 rxns; PN 1000298</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000366</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 4 rxns; PN 1000265</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000340</t>
   </si>
   <si>
-    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000261</t>
-  </si>
-  <si>
-    <t>Parse Biosciences; Evercode WT v2 Kit, 48 rxns; PN ECW02030</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000341</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 16 rxns; PN 1000263</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000339</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns PN 1000092</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
   </si>
   <si>
-    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 16 rxns; PN 1000268</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000337</t>
-  </si>
-  <si>
     <t>Custom</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000335</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN 120267</t>
   </si>
   <si>
@@ -1449,54 +1500,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000355</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell 3' GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
   </si>
   <si>
-    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000322</t>
-  </si>
-  <si>
-    <t>Illumina; TruSeq Stranded mRNA Library Prep (48 samples); PN 20020594</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000343</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 24 rxns; PN 1000290</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000365</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 4 rxns; PN 1000269</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000338</t>
   </si>
   <si>
-    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
-  </si>
-  <si>
-    <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000342</t>
-  </si>
-  <si>
     <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
   </si>
   <si>
@@ -1779,12 +1794,6 @@
     <t>https://identifiers.org/RRID:SCR_023729</t>
   </si>
   <si>
-    <t>EVOS M7000</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_025070</t>
-  </si>
-  <si>
     <t>Chromium Controller</t>
   </si>
   <si>
@@ -1854,6 +1863,12 @@
     <t>preparation_instrument_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip K Automated Single Cell Kit, 48 rxns; PN 1000289</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000373</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Chip K Single Cell Kit, 48 rxns; PN 1000286</t>
   </si>
   <si>
@@ -1896,7 +1911,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-22T07:33:22-07:00</t>
+    <t>2024-03-25T11:33:15-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2100,124 +2115,124 @@
         <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2">
@@ -2225,7 +2240,7 @@
         <v>52</v>
       </c>
       <c r="AV2" t="s" s="49">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -2243,7 +2258,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2260,7 +2275,7 @@
       <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_offset'!$A$1:$A$7</formula1>
+      <formula1>'barcode_offset'!$A$1:$A$8</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'barcode_read'!$A$1:$A$3</formula1>
@@ -2328,7 +2343,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$24</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$25</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$15</formula1>
@@ -2350,7 +2365,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$17</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$6</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2369,26 +2384,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2406,32 +2421,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2449,22 +2464,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2482,26 +2497,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2519,27 +2534,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2557,42 +2572,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2610,18 +2625,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2639,18 +2654,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2668,18 +2683,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2697,18 +2712,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3011,18 +3026,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3032,7 +3047,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3040,194 +3055,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>370</v>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>374</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3245,122 +3268,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>379</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>387</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>391</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>399</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -3401,178 +3424,178 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>405</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>425</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>427</v>
+        <v>432</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>429</v>
+        <v>434</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>435</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>445</v>
+        <v>450</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -3606,10 +3629,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4">
@@ -3622,26 +3645,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>455</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>457</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8">
@@ -3654,10 +3677,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -3675,138 +3698,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>151</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>462</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>463</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>464</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>219</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -3816,7 +3839,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3824,50 +3847,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>335</v>
+        <v>491</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>336</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>488</v>
+        <v>370</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>489</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>495</v>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>499</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -3891,16 +3922,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
@@ -3908,13 +3939,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -4237,7 +4268,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4625,6 +4656,14 @@
       </c>
       <c r="B48" t="s" s="0">
         <v>239</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4642,42 +4681,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -4695,26 +4734,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4724,7 +4763,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4732,37 +4771,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new categorical values
Closes #23
</commit_message>
<xml_diff>
--- a/rnaseq/latest/rnaseq.xlsx
+++ b/rnaseq/latest/rnaseq.xlsx
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="512">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1848,6 +1848,12 @@
     <t>https://identifiers.org/RRID:SCR_024536</t>
   </si>
   <si>
+    <t>Chromium Connect</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025146</t>
+  </si>
+  <si>
     <t>M5 Sprayer</t>
   </si>
   <si>
@@ -1911,7 +1917,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-25T11:33:15-07:00</t>
+    <t>2024-03-26T13:37:42-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2229,10 +2235,10 @@
         <v>465</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="2">
@@ -2240,7 +2246,7 @@
         <v>52</v>
       </c>
       <c r="AV2" t="s" s="49">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -2362,7 +2368,7 @@
       <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AT2:AT1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$17</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_kit'!$A$1:$A$7</formula1>
@@ -3690,7 +3696,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3830,6 +3836,14 @@
       </c>
       <c r="B17" t="s" s="0">
         <v>489</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -3847,10 +3861,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2">
@@ -3871,34 +3885,34 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -3922,16 +3936,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="2">
@@ -3939,13 +3953,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new preparation instrument kits and library preparation kit
Closes #28
</commit_message>
<xml_diff>
--- a/rnaseq/latest/rnaseq.xlsx
+++ b/rnaseq/latest/rnaseq.xlsx
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="526">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1458,6 +1458,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000374</t>
   </si>
   <si>
+    <t>New England BioLabs; NEBNext Ultra II RNA Library Prep Kit for Illumina; PN E7770</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000377</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 24 rxns; PN 1000290</t>
   </si>
   <si>
@@ -1500,6 +1506,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Hybridization &amp; Library Kit, 4 rxns; PN 1000415</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000375</t>
+  </si>
+  <si>
     <t>Custom</t>
   </si>
   <si>
@@ -1887,6 +1899,12 @@
     <t>preparation_instrument_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip G Single Cell Kit, 16 rxns; PN 1000127</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000379</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Chip K Automated Single Cell Kit, 48 rxns; PN 1000289</t>
   </si>
   <si>
@@ -1899,6 +1917,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000367</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip G Single Cell Kit, 48 rxns; PN 1000120</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000378</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium FFPE Reagent Kit v2-Small, PN 1000436</t>
   </si>
   <si>
@@ -1935,7 +1959,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-01T14:49:27-07:00</t>
+    <t>2024-04-05T13:06:18-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2223,40 +2247,40 @@
         <v>331</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>509</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2">
@@ -2264,7 +2288,7 @@
         <v>52</v>
       </c>
       <c r="AV2" t="s" s="49">
-        <v>510</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -2367,7 +2391,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$25</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$15</formula1>
@@ -2389,7 +2413,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$7</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3071,7 +3095,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3275,6 +3299,22 @@
       </c>
       <c r="B25" t="s" s="0">
         <v>381</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>382</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>384</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -3292,10 +3332,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2">
@@ -3308,106 +3348,106 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -3448,178 +3488,178 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -3669,26 +3709,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8">
@@ -3701,10 +3741,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -3738,10 +3778,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4">
@@ -3754,10 +3794,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6">
@@ -3778,90 +3818,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -3871,7 +3911,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3879,58 +3919,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>376</v>
+        <v>505</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>377</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>367</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>501</v>
+        <v>368</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>502</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>508</v>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>513</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>515</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -3954,16 +4010,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>516</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2">
@@ -3971,13 +4027,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>517</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new library preparation kit and sample indexing kit
Closes #33 and closes #35
</commit_message>
<xml_diff>
--- a/rnaseq/latest/rnaseq.xlsx
+++ b/rnaseq/latest/rnaseq.xlsx
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="530">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1569,6 +1569,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000348</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium i7 Sample Index Plate (96 rxn); PN 220103</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000380</t>
+  </si>
+  <si>
     <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-AB</t>
   </si>
   <si>
@@ -1755,6 +1761,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
   </si>
   <si>
+    <t>Illumina; NextSeq 500/550 Hi Output Kit 75 Cycles v2.5; PN 20024906</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000381</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles); PN 20028312</t>
   </si>
   <si>
@@ -1959,7 +1971,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-05T13:06:18-07:00</t>
+    <t>2024-04-20T17:33:01-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2250,37 +2262,37 @@
         <v>386</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2">
@@ -2288,7 +2300,7 @@
         <v>52</v>
       </c>
       <c r="AV2" t="s" s="49">
-        <v>518</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -2394,7 +2406,7 @@
       <formula1>'library_preparation_kit'!$A$1:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sample_indexing_kit'!$A$1:$A$15</formula1>
+      <formula1>'sample_indexing_kit'!$A$1:$A$16</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AM2:AM1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_technical_replicate'!$A$1:$A$2</formula1>
@@ -2404,7 +2416,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AO2:AO1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$22</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
@@ -3324,7 +3336,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3448,6 +3460,14 @@
       </c>
       <c r="B15" t="s" s="0">
         <v>414</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>415</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3480,7 +3500,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3488,178 +3508,186 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>462</v>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>465</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -3709,26 +3737,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8">
@@ -3741,10 +3769,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -3778,10 +3806,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="4">
@@ -3794,10 +3822,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6">
@@ -3818,90 +3846,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>499</v>
+        <v>503</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -3919,18 +3947,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3">
@@ -3951,42 +3979,42 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>510</v>
+        <v>514</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>512</v>
+        <v>516</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -4010,16 +4038,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2">
@@ -4027,13 +4055,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>